<commit_message>
mise a jour devis
</commit_message>
<xml_diff>
--- a/Projet-location-velo/Devis.xlsx
+++ b/Projet-location-velo/Devis.xlsx
@@ -41,12 +41,6 @@
     <t>Graphiste</t>
   </si>
   <si>
-    <t>Chef de projet</t>
-  </si>
-  <si>
-    <t>Développeur</t>
-  </si>
-  <si>
     <t>DESIGNATION</t>
   </si>
   <si>
@@ -75,6 +69,12 @@
   </si>
   <si>
     <t>UNITE</t>
+  </si>
+  <si>
+    <t>Développement</t>
+  </si>
+  <si>
+    <t>Pôle Validation</t>
   </si>
 </sst>
 </file>
@@ -355,6 +355,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -363,10 +367,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -652,7 +652,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,26 +664,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -763,22 +763,22 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5">
         <v>600</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B10" s="15">
         <v>20</v>
@@ -792,37 +792,37 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>15</v>
+      <c r="A11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="10"/>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="8">
         <f>SUM(D4:D12)</f>
-        <v>10470</v>
+        <v>9270</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="6">
         <v>0</v>
@@ -832,11 +832,11 @@
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="9">
         <f>SUM(D13)</f>
-        <v>10470</v>
+        <v>9270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>